<commit_message>
'xlsxwriter' engine for ExtelWriter; additional data
</commit_message>
<xml_diff>
--- a/disk_savvy.xlsx
+++ b/disk_savvy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\NAUKA\Python Nauka\data_science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CB9790-D0E9-441B-824A-67A4863D2D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD23D2E4-9521-4B03-80CF-9A16E7B21B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="624" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13440" yWindow="1848" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -356,9 +356,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -897,6 +899,20 @@
         <v>684.06</v>
       </c>
     </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>44695</v>
+      </c>
+      <c r="B39" s="2">
+        <v>0.71908564814814813</v>
+      </c>
+      <c r="C39">
+        <v>36207</v>
+      </c>
+      <c r="D39">
+        <v>685.19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
mainly whole plots_from_web directory
</commit_message>
<xml_diff>
--- a/disk_savvy.xlsx
+++ b/disk_savvy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\NAUKA\Python Nauka\data_science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD23D2E4-9521-4B03-80CF-9A16E7B21B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF90225E-4A43-47A3-ADBA-7676157CD5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13440" yWindow="1848" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4530" yWindow="2910" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -356,18 +356,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -381,7 +381,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44666</v>
       </c>
@@ -395,7 +395,7 @@
         <v>94.96</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44666</v>
       </c>
@@ -409,7 +409,7 @@
         <v>190.21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44666</v>
       </c>
@@ -423,7 +423,7 @@
         <v>306.95999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44666</v>
       </c>
@@ -437,7 +437,7 @@
         <v>368.45</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44666</v>
       </c>
@@ -451,7 +451,7 @@
         <v>388.04</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44666</v>
       </c>
@@ -465,7 +465,7 @@
         <v>389.08</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44666</v>
       </c>
@@ -479,7 +479,7 @@
         <v>394.11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44666</v>
       </c>
@@ -493,7 +493,7 @@
         <v>443.43</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44666</v>
       </c>
@@ -507,7 +507,7 @@
         <v>444.97</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44666</v>
       </c>
@@ -521,7 +521,7 @@
         <v>451.99</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44666</v>
       </c>
@@ -535,7 +535,7 @@
         <v>454.26</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44666</v>
       </c>
@@ -549,7 +549,7 @@
         <v>465.72</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44669</v>
       </c>
@@ -563,7 +563,7 @@
         <v>484.07</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44669</v>
       </c>
@@ -577,7 +577,7 @@
         <v>484.1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44669</v>
       </c>
@@ -591,7 +591,7 @@
         <v>484.2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44669</v>
       </c>
@@ -605,7 +605,7 @@
         <v>484.45</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44670</v>
       </c>
@@ -619,7 +619,7 @@
         <v>528.97</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44671</v>
       </c>
@@ -633,7 +633,7 @@
         <v>529.36</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44672</v>
       </c>
@@ -647,7 +647,7 @@
         <v>569.15</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44673</v>
       </c>
@@ -661,7 +661,7 @@
         <v>569.34</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44674</v>
       </c>
@@ -675,7 +675,7 @@
         <v>605.58000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44674</v>
       </c>
@@ -689,7 +689,7 @@
         <v>657.97</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44675</v>
       </c>
@@ -703,7 +703,7 @@
         <v>666.9</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44675</v>
       </c>
@@ -717,7 +717,7 @@
         <v>667.04</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44676</v>
       </c>
@@ -731,7 +731,7 @@
         <v>669.67</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44676</v>
       </c>
@@ -745,7 +745,7 @@
         <v>669.65</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44677</v>
       </c>
@@ -759,7 +759,7 @@
         <v>670.34</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44678</v>
       </c>
@@ -773,7 +773,7 @@
         <v>670.14</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44679</v>
       </c>
@@ -787,7 +787,7 @@
         <v>670.09</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44679</v>
       </c>
@@ -801,7 +801,7 @@
         <v>670.1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44683</v>
       </c>
@@ -815,7 +815,7 @@
         <v>676.09</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44684</v>
       </c>
@@ -829,7 +829,7 @@
         <v>676.12</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44686</v>
       </c>
@@ -843,7 +843,7 @@
         <v>676.14</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44690</v>
       </c>
@@ -857,7 +857,7 @@
         <v>676.15</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44692</v>
       </c>
@@ -871,7 +871,7 @@
         <v>682.72</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44692</v>
       </c>
@@ -885,7 +885,7 @@
         <v>682.82</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44693</v>
       </c>
@@ -899,7 +899,7 @@
         <v>684.06</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44695</v>
       </c>
@@ -911,6 +911,258 @@
       </c>
       <c r="D39">
         <v>685.19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>44697</v>
+      </c>
+      <c r="B40" s="2">
+        <v>0.63185185185185189</v>
+      </c>
+      <c r="C40">
+        <v>36208</v>
+      </c>
+      <c r="D40">
+        <v>685.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>44697</v>
+      </c>
+      <c r="B41" s="2">
+        <v>0.6348611111111111</v>
+      </c>
+      <c r="C41">
+        <v>36201</v>
+      </c>
+      <c r="D41">
+        <v>685.21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>44697</v>
+      </c>
+      <c r="B42" s="2">
+        <v>0.96414351851851843</v>
+      </c>
+      <c r="C42">
+        <v>36204</v>
+      </c>
+      <c r="D42">
+        <v>685.22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>44698</v>
+      </c>
+      <c r="B43" s="2">
+        <v>0.40944444444444444</v>
+      </c>
+      <c r="C43">
+        <v>36252</v>
+      </c>
+      <c r="D43">
+        <v>685.72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>44698</v>
+      </c>
+      <c r="B44" s="2">
+        <v>0.99490740740740735</v>
+      </c>
+      <c r="C44">
+        <v>36250</v>
+      </c>
+      <c r="D44">
+        <v>684.67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>44699</v>
+      </c>
+      <c r="B45" s="2">
+        <v>0.93873842592592593</v>
+      </c>
+      <c r="C45">
+        <v>36254</v>
+      </c>
+      <c r="D45">
+        <v>684.85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>44700</v>
+      </c>
+      <c r="B46" s="2">
+        <v>0.48609953703703707</v>
+      </c>
+      <c r="C46">
+        <v>36248</v>
+      </c>
+      <c r="D46">
+        <v>684.7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>44700</v>
+      </c>
+      <c r="B47" s="2">
+        <v>0.98951388888888892</v>
+      </c>
+      <c r="C47">
+        <v>36248</v>
+      </c>
+      <c r="D47">
+        <v>684.81</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>44701</v>
+      </c>
+      <c r="B48" s="2">
+        <v>0.99653935185185183</v>
+      </c>
+      <c r="C48">
+        <v>36250</v>
+      </c>
+      <c r="D48">
+        <v>684.78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>44704</v>
+      </c>
+      <c r="B49" s="2">
+        <v>0.64586805555555549</v>
+      </c>
+      <c r="C49">
+        <v>36250</v>
+      </c>
+      <c r="D49">
+        <v>684.79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>44706</v>
+      </c>
+      <c r="B50" s="2">
+        <v>0.56009259259259259</v>
+      </c>
+      <c r="C50">
+        <v>36250</v>
+      </c>
+      <c r="D50">
+        <v>684.8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>44712</v>
+      </c>
+      <c r="B51" s="2">
+        <v>0.47394675925925928</v>
+      </c>
+      <c r="C51">
+        <v>36253</v>
+      </c>
+      <c r="D51">
+        <v>684.81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B52" s="2">
+        <v>0.65696759259259252</v>
+      </c>
+      <c r="C52">
+        <v>36259</v>
+      </c>
+      <c r="D52">
+        <v>684.98</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>44715</v>
+      </c>
+      <c r="B53" s="2">
+        <v>0.53877314814814814</v>
+      </c>
+      <c r="C53">
+        <v>36259</v>
+      </c>
+      <c r="D53">
+        <v>685.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>44723</v>
+      </c>
+      <c r="B54" s="2">
+        <v>0.46240740740740738</v>
+      </c>
+      <c r="C54">
+        <v>36231</v>
+      </c>
+      <c r="D54">
+        <v>685.14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>44766</v>
+      </c>
+      <c r="B55" s="2">
+        <v>0.85538194444444438</v>
+      </c>
+      <c r="C55">
+        <v>36354</v>
+      </c>
+      <c r="D55">
+        <v>685.55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>44769</v>
+      </c>
+      <c r="B56" s="2">
+        <v>0.93134259259259267</v>
+      </c>
+      <c r="C56">
+        <v>70024</v>
+      </c>
+      <c r="D56">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>44771</v>
+      </c>
+      <c r="B57" s="2">
+        <v>0.76491898148148152</v>
+      </c>
+      <c r="C57">
+        <v>71693</v>
+      </c>
+      <c r="D57">
+        <v>1190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
twitch stats, supremacy, disk analysis
</commit_message>
<xml_diff>
--- a/disk_savvy.xlsx
+++ b/disk_savvy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\NAUKA\Python Nauka\data_science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBFCB24-879B-4468-9953-3896B11C4947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66E7C14-7635-4C2C-9E65-EFD78330CC8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="408" windowWidth="11520" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -356,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1347,6 +1347,20 @@
         <v>1430</v>
       </c>
     </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
+        <v>45021</v>
+      </c>
+      <c r="B71" s="2">
+        <v>0.33241898148148147</v>
+      </c>
+      <c r="C71">
+        <v>75499</v>
+      </c>
+      <c r="D71">
+        <v>1430</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more data; data extraction for supremacy
</commit_message>
<xml_diff>
--- a/disk_savvy.xlsx
+++ b/disk_savvy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\NAUKA\Python Nauka\data_science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331E60E6-17D0-49BF-9284-38C3473E4124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17843B58-5416-455C-80F1-5A6DAA27636B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="408" windowWidth="11520" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -356,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1389,6 +1389,34 @@
         <v>1430</v>
       </c>
     </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
+        <v>45031</v>
+      </c>
+      <c r="B74" s="2">
+        <v>0.8175810185185185</v>
+      </c>
+      <c r="C74">
+        <v>75573</v>
+      </c>
+      <c r="D74">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
+        <v>41382</v>
+      </c>
+      <c r="B75" s="2">
+        <v>0.65328703703703705</v>
+      </c>
+      <c r="C75">
+        <v>75573</v>
+      </c>
+      <c r="D75">
+        <v>1430</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more supremacy1914 and disk_savvy data
</commit_message>
<xml_diff>
--- a/disk_savvy.xlsx
+++ b/disk_savvy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\NAUKA\Python Nauka\data_science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17843B58-5416-455C-80F1-5A6DAA27636B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753DE795-6ADA-431F-9745-A86501D6EAE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="408" windowWidth="11520" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-405" yWindow="2640" windowWidth="5490" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -356,18 +356,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -381,7 +381,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44666</v>
       </c>
@@ -395,7 +395,7 @@
         <v>94.96</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44666</v>
       </c>
@@ -409,7 +409,7 @@
         <v>190.21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44666</v>
       </c>
@@ -423,7 +423,7 @@
         <v>306.95999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44666</v>
       </c>
@@ -437,7 +437,7 @@
         <v>368.45</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44666</v>
       </c>
@@ -451,7 +451,7 @@
         <v>388.04</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44666</v>
       </c>
@@ -465,7 +465,7 @@
         <v>389.08</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44666</v>
       </c>
@@ -479,7 +479,7 @@
         <v>394.11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44666</v>
       </c>
@@ -493,7 +493,7 @@
         <v>443.43</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44666</v>
       </c>
@@ -507,7 +507,7 @@
         <v>444.97</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44666</v>
       </c>
@@ -521,7 +521,7 @@
         <v>451.99</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44666</v>
       </c>
@@ -535,7 +535,7 @@
         <v>454.26</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44666</v>
       </c>
@@ -549,7 +549,7 @@
         <v>465.72</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44669</v>
       </c>
@@ -563,7 +563,7 @@
         <v>484.07</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44669</v>
       </c>
@@ -577,7 +577,7 @@
         <v>484.1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44669</v>
       </c>
@@ -591,7 +591,7 @@
         <v>484.2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44669</v>
       </c>
@@ -605,7 +605,7 @@
         <v>484.45</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44670</v>
       </c>
@@ -619,7 +619,7 @@
         <v>528.97</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44671</v>
       </c>
@@ -633,7 +633,7 @@
         <v>529.36</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44672</v>
       </c>
@@ -647,7 +647,7 @@
         <v>569.15</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44673</v>
       </c>
@@ -661,7 +661,7 @@
         <v>569.34</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44674</v>
       </c>
@@ -675,7 +675,7 @@
         <v>605.58000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44674</v>
       </c>
@@ -689,7 +689,7 @@
         <v>657.97</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44675</v>
       </c>
@@ -703,7 +703,7 @@
         <v>666.9</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44675</v>
       </c>
@@ -717,7 +717,7 @@
         <v>667.04</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44676</v>
       </c>
@@ -731,7 +731,7 @@
         <v>669.67</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44676</v>
       </c>
@@ -745,7 +745,7 @@
         <v>669.65</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44677</v>
       </c>
@@ -759,7 +759,7 @@
         <v>670.34</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44678</v>
       </c>
@@ -773,7 +773,7 @@
         <v>670.14</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44679</v>
       </c>
@@ -787,7 +787,7 @@
         <v>670.09</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44679</v>
       </c>
@@ -801,7 +801,7 @@
         <v>670.1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44683</v>
       </c>
@@ -815,7 +815,7 @@
         <v>676.09</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44684</v>
       </c>
@@ -829,7 +829,7 @@
         <v>676.12</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44686</v>
       </c>
@@ -843,7 +843,7 @@
         <v>676.14</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44690</v>
       </c>
@@ -857,7 +857,7 @@
         <v>676.15</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44692</v>
       </c>
@@ -871,7 +871,7 @@
         <v>682.72</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44692</v>
       </c>
@@ -885,7 +885,7 @@
         <v>682.82</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44693</v>
       </c>
@@ -899,7 +899,7 @@
         <v>684.06</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44695</v>
       </c>
@@ -913,7 +913,7 @@
         <v>685.19</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44697</v>
       </c>
@@ -927,7 +927,7 @@
         <v>685.2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44697</v>
       </c>
@@ -941,7 +941,7 @@
         <v>685.21</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44697</v>
       </c>
@@ -955,7 +955,7 @@
         <v>685.22</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44698</v>
       </c>
@@ -969,7 +969,7 @@
         <v>685.72</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44698</v>
       </c>
@@ -983,7 +983,7 @@
         <v>684.67</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44699</v>
       </c>
@@ -997,7 +997,7 @@
         <v>684.85</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44700</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>684.7</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44700</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>684.81</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44701</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>684.78</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44704</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>684.79</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44706</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>684.8</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44712</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>684.81</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44713</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>684.98</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44715</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>685.1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44723</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>685.14</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44766</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>685.55</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44769</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44771</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44872</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44568</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>45007</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>45007</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>1410</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>45007</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>1410</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>45009</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>45011</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>45013</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>45015</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>45016</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>45017</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>45018</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>45019</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>45021</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>45025</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>45027</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>45031</v>
       </c>
@@ -1403,9 +1403,9 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>41382</v>
+        <v>45034</v>
       </c>
       <c r="B75" s="2">
         <v>0.65328703703703705</v>
@@ -1415,6 +1415,34 @@
       </c>
       <c r="D75">
         <v>1430</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>45088</v>
+      </c>
+      <c r="B76" s="2">
+        <v>0.44122685185185184</v>
+      </c>
+      <c r="C76">
+        <v>77494</v>
+      </c>
+      <c r="D76">
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>45091</v>
+      </c>
+      <c r="B77" s="2">
+        <v>0.44196759259259261</v>
+      </c>
+      <c r="C77">
+        <v>81206</v>
+      </c>
+      <c r="D77">
+        <v>1620</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sullygnome, supremacy, packages update. Seaborn datasets analysis.
</commit_message>
<xml_diff>
--- a/disk_savvy.xlsx
+++ b/disk_savvy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\NAUKA\Python Nauka\data_science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753DE795-6ADA-431F-9745-A86501D6EAE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4989540B-5402-4FD0-88FF-10A8BAA93A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-405" yWindow="2640" windowWidth="5490" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="5490" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -356,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1445,6 +1445,412 @@
         <v>1620</v>
       </c>
     </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>45094</v>
+      </c>
+      <c r="B78" s="2">
+        <v>0.72203703703703714</v>
+      </c>
+      <c r="C78">
+        <v>81200</v>
+      </c>
+      <c r="D78">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>45096</v>
+      </c>
+      <c r="B79" s="2">
+        <v>0.42538194444444444</v>
+      </c>
+      <c r="C79">
+        <v>81201</v>
+      </c>
+      <c r="D79">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>45097</v>
+      </c>
+      <c r="B80" s="2">
+        <v>0.71953703703703698</v>
+      </c>
+      <c r="C80">
+        <v>81203</v>
+      </c>
+      <c r="D80">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>45098</v>
+      </c>
+      <c r="B81" s="2">
+        <v>0.89884259259259258</v>
+      </c>
+      <c r="C81">
+        <v>81219</v>
+      </c>
+      <c r="D81">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>45099</v>
+      </c>
+      <c r="B82" s="2">
+        <v>0.67739583333333331</v>
+      </c>
+      <c r="C82">
+        <v>81221</v>
+      </c>
+      <c r="D82">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>45101</v>
+      </c>
+      <c r="B83" s="2">
+        <v>0.52664351851851854</v>
+      </c>
+      <c r="C83">
+        <v>81218</v>
+      </c>
+      <c r="D83">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>45102</v>
+      </c>
+      <c r="B84" s="2">
+        <v>0.46377314814814818</v>
+      </c>
+      <c r="C84">
+        <v>81256</v>
+      </c>
+      <c r="D84">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>45104</v>
+      </c>
+      <c r="B85" s="2">
+        <v>0.47160879629629626</v>
+      </c>
+      <c r="C85">
+        <v>81288</v>
+      </c>
+      <c r="D85">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>45105</v>
+      </c>
+      <c r="B86" s="2">
+        <v>0.47478009259259263</v>
+      </c>
+      <c r="C86">
+        <v>81310</v>
+      </c>
+      <c r="D86">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>45106</v>
+      </c>
+      <c r="B87" s="2">
+        <v>0.76927083333333324</v>
+      </c>
+      <c r="C87">
+        <v>81300</v>
+      </c>
+      <c r="D87">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B88" s="2">
+        <v>0.64849537037037031</v>
+      </c>
+      <c r="C88">
+        <v>81371</v>
+      </c>
+      <c r="D88">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>45108</v>
+      </c>
+      <c r="B89" s="2">
+        <v>0.68618055555555557</v>
+      </c>
+      <c r="C89">
+        <v>81495</v>
+      </c>
+      <c r="D89">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>45109</v>
+      </c>
+      <c r="B90" s="2">
+        <v>0.60706018518518523</v>
+      </c>
+      <c r="C90">
+        <v>81495</v>
+      </c>
+      <c r="D90">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>45110</v>
+      </c>
+      <c r="B91" s="2">
+        <v>0.47806712962962966</v>
+      </c>
+      <c r="C91">
+        <v>81494</v>
+      </c>
+      <c r="D91">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>45111</v>
+      </c>
+      <c r="B92" s="2">
+        <v>0.38723379629629634</v>
+      </c>
+      <c r="C92">
+        <v>81494</v>
+      </c>
+      <c r="D92">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>45112</v>
+      </c>
+      <c r="B93" s="2">
+        <v>0.45993055555555556</v>
+      </c>
+      <c r="C93">
+        <v>81498</v>
+      </c>
+      <c r="D93">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>45113</v>
+      </c>
+      <c r="B94" s="2">
+        <v>0.44883101851851853</v>
+      </c>
+      <c r="C94">
+        <v>81507</v>
+      </c>
+      <c r="D94">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>45114</v>
+      </c>
+      <c r="B95" s="2">
+        <v>0.48599537037037038</v>
+      </c>
+      <c r="C95">
+        <v>81618</v>
+      </c>
+      <c r="D95">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>45115</v>
+      </c>
+      <c r="B96" s="2">
+        <v>0.46984953703703702</v>
+      </c>
+      <c r="C96">
+        <v>81618</v>
+      </c>
+      <c r="D96">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>45116</v>
+      </c>
+      <c r="B97" s="2">
+        <v>0.46643518518518517</v>
+      </c>
+      <c r="C97">
+        <v>81620</v>
+      </c>
+      <c r="D97">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>45117</v>
+      </c>
+      <c r="B98" s="2">
+        <v>0.46270833333333333</v>
+      </c>
+      <c r="C98">
+        <v>81620</v>
+      </c>
+      <c r="D98">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>45118</v>
+      </c>
+      <c r="B99" s="2">
+        <v>0.5430787037037037</v>
+      </c>
+      <c r="C99">
+        <v>81620</v>
+      </c>
+      <c r="D99">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>45119</v>
+      </c>
+      <c r="B100" s="2">
+        <v>0.46430555555555553</v>
+      </c>
+      <c r="C100">
+        <v>81610</v>
+      </c>
+      <c r="D100">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>45120</v>
+      </c>
+      <c r="B101" s="2">
+        <v>0.50746527777777783</v>
+      </c>
+      <c r="C101">
+        <v>81612</v>
+      </c>
+      <c r="D101">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>45121</v>
+      </c>
+      <c r="B102" s="2">
+        <v>0.58672453703703698</v>
+      </c>
+      <c r="C102">
+        <v>81613</v>
+      </c>
+      <c r="D102">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>45122</v>
+      </c>
+      <c r="B103" s="2">
+        <v>0.51321759259259259</v>
+      </c>
+      <c r="C103">
+        <v>81615</v>
+      </c>
+      <c r="D103">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>45123</v>
+      </c>
+      <c r="B104" s="2">
+        <v>0.5237384259259259</v>
+      </c>
+      <c r="C104">
+        <v>81615</v>
+      </c>
+      <c r="D104">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>45124</v>
+      </c>
+      <c r="B105" s="2">
+        <v>0.50491898148148151</v>
+      </c>
+      <c r="C105">
+        <v>81615</v>
+      </c>
+      <c r="D105">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>45125</v>
+      </c>
+      <c r="B106" s="2">
+        <v>0.47068287037037032</v>
+      </c>
+      <c r="C106">
+        <v>81637</v>
+      </c>
+      <c r="D106">
+        <v>1630</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
packages update. Seaborn datasets analysis.
</commit_message>
<xml_diff>
--- a/disk_savvy.xlsx
+++ b/disk_savvy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\NAUKA\Python Nauka\data_science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4989540B-5402-4FD0-88FF-10A8BAA93A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6179D0BA-36B8-4F39-B153-A2755B313248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="5490" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -356,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D106"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1851,6 +1851,104 @@
         <v>1630</v>
       </c>
     </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>45126</v>
+      </c>
+      <c r="B107" s="2">
+        <v>0.68236111111111108</v>
+      </c>
+      <c r="C107">
+        <v>81639</v>
+      </c>
+      <c r="D107">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>45127</v>
+      </c>
+      <c r="B108" s="2">
+        <v>0.45068287037037041</v>
+      </c>
+      <c r="C108">
+        <v>83211</v>
+      </c>
+      <c r="D108">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>45128</v>
+      </c>
+      <c r="B109" s="2">
+        <v>0.48158564814814814</v>
+      </c>
+      <c r="C109">
+        <v>83215</v>
+      </c>
+      <c r="D109">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>45129</v>
+      </c>
+      <c r="B110" s="2">
+        <v>0.58716435185185178</v>
+      </c>
+      <c r="C110">
+        <v>83215</v>
+      </c>
+      <c r="D110">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>45130</v>
+      </c>
+      <c r="B111" s="2">
+        <v>0.47083333333333338</v>
+      </c>
+      <c r="C111">
+        <v>83215</v>
+      </c>
+      <c r="D111">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>45131</v>
+      </c>
+      <c r="B112" s="2">
+        <v>0.51880787037037035</v>
+      </c>
+      <c r="C112">
+        <v>83217</v>
+      </c>
+      <c r="D112">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>45132</v>
+      </c>
+      <c r="B113" s="2">
+        <v>0.60712962962962969</v>
+      </c>
+      <c r="C113">
+        <v>83217</v>
+      </c>
+      <c r="D113">
+        <v>1680</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
więcej danych disk_savvy; analiza sns datasets
</commit_message>
<xml_diff>
--- a/disk_savvy.xlsx
+++ b/disk_savvy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\NAUKA\Python Nauka\data_science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6179D0BA-36B8-4F39-B153-A2755B313248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F1D72E-1DBA-4F69-ADB8-3F4DDC0C0ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="5490" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -356,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D113"/>
+  <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A121" sqref="A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1949,6 +1949,104 @@
         <v>1680</v>
       </c>
     </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>45133</v>
+      </c>
+      <c r="B114" s="2">
+        <v>0.46194444444444444</v>
+      </c>
+      <c r="C114">
+        <v>83219</v>
+      </c>
+      <c r="D114">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>45134</v>
+      </c>
+      <c r="B115" s="2">
+        <v>0.89277777777777778</v>
+      </c>
+      <c r="C115">
+        <v>83220</v>
+      </c>
+      <c r="D115">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>45135</v>
+      </c>
+      <c r="B116" s="2">
+        <v>0.75491898148148151</v>
+      </c>
+      <c r="C116">
+        <v>83220</v>
+      </c>
+      <c r="D116">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <v>45136</v>
+      </c>
+      <c r="B117" s="2">
+        <v>0.58952546296296293</v>
+      </c>
+      <c r="C117">
+        <v>83236</v>
+      </c>
+      <c r="D117">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>45137</v>
+      </c>
+      <c r="B118" s="2">
+        <v>0.4776157407407407</v>
+      </c>
+      <c r="C118">
+        <v>83236</v>
+      </c>
+      <c r="D118">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>45138</v>
+      </c>
+      <c r="B119" s="2">
+        <v>0.4611574074074074</v>
+      </c>
+      <c r="C119">
+        <v>83236</v>
+      </c>
+      <c r="D119">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>45139</v>
+      </c>
+      <c r="B120" s="2">
+        <v>0.46293981481481478</v>
+      </c>
+      <c r="C120">
+        <v>83244</v>
+      </c>
+      <c r="D120">
+        <v>1690</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
więcej disk_savvy, sullygnome oraz analiza sns.datasets
</commit_message>
<xml_diff>
--- a/disk_savvy.xlsx
+++ b/disk_savvy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\NAUKA\Python Nauka\data_science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F1D72E-1DBA-4F69-ADB8-3F4DDC0C0ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49162ACC-BDF3-41E6-8474-E396535D9318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="5490" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -356,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D120"/>
+  <dimension ref="A1:D136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A121" sqref="A121"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="A137" sqref="A137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2047,6 +2047,230 @@
         <v>1690</v>
       </c>
     </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>45140</v>
+      </c>
+      <c r="B121" s="2">
+        <v>0.54917824074074073</v>
+      </c>
+      <c r="C121">
+        <v>83247</v>
+      </c>
+      <c r="D121">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>45141</v>
+      </c>
+      <c r="B122" s="2">
+        <v>0.64541666666666664</v>
+      </c>
+      <c r="C122">
+        <v>83254</v>
+      </c>
+      <c r="D122">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <v>45142</v>
+      </c>
+      <c r="B123" s="2">
+        <v>0.43209490740740741</v>
+      </c>
+      <c r="C123">
+        <v>83255</v>
+      </c>
+      <c r="D123">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <v>45143</v>
+      </c>
+      <c r="B124" s="2">
+        <v>0.47541666666666665</v>
+      </c>
+      <c r="C124">
+        <v>83255</v>
+      </c>
+      <c r="D124">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>45144</v>
+      </c>
+      <c r="B125" s="2">
+        <v>0.4729976851851852</v>
+      </c>
+      <c r="C125">
+        <v>83255</v>
+      </c>
+      <c r="D125">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>45145</v>
+      </c>
+      <c r="B126" s="2">
+        <v>0.4765625</v>
+      </c>
+      <c r="C126">
+        <v>83280</v>
+      </c>
+      <c r="D126">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>45146</v>
+      </c>
+      <c r="B127" s="2">
+        <v>0.46464120370370371</v>
+      </c>
+      <c r="C127">
+        <v>83280</v>
+      </c>
+      <c r="D127">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>45147</v>
+      </c>
+      <c r="B128" s="2">
+        <v>0.36782407407407408</v>
+      </c>
+      <c r="C128">
+        <v>83284</v>
+      </c>
+      <c r="D128">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>45148</v>
+      </c>
+      <c r="B129" s="2">
+        <v>0.48040509259259262</v>
+      </c>
+      <c r="C129">
+        <v>83287</v>
+      </c>
+      <c r="D129">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>45149</v>
+      </c>
+      <c r="B130" s="2">
+        <v>0.52964120370370371</v>
+      </c>
+      <c r="C130">
+        <v>83291</v>
+      </c>
+      <c r="D130">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>45150</v>
+      </c>
+      <c r="B131" s="2">
+        <v>0.47501157407407407</v>
+      </c>
+      <c r="C131">
+        <v>83359</v>
+      </c>
+      <c r="D131">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>45151</v>
+      </c>
+      <c r="B132" s="2">
+        <v>0.46175925925925926</v>
+      </c>
+      <c r="C132">
+        <v>83359</v>
+      </c>
+      <c r="D132">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>45152</v>
+      </c>
+      <c r="B133" s="2">
+        <v>0.46082175925925922</v>
+      </c>
+      <c r="C133">
+        <v>83359</v>
+      </c>
+      <c r="D133">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>45153</v>
+      </c>
+      <c r="B134" s="2">
+        <v>0.39368055555555559</v>
+      </c>
+      <c r="C134">
+        <v>83359</v>
+      </c>
+      <c r="D134">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>45154</v>
+      </c>
+      <c r="B135" s="2">
+        <v>0.41212962962962968</v>
+      </c>
+      <c r="C135">
+        <v>83360</v>
+      </c>
+      <c r="D135">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>45155</v>
+      </c>
+      <c r="B136" s="2">
+        <v>0.42332175925925924</v>
+      </c>
+      <c r="C136">
+        <v>77977</v>
+      </c>
+      <c r="D136">
+        <v>1680</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more data for 'disc_savvy'
</commit_message>
<xml_diff>
--- a/disk_savvy.xlsx
+++ b/disk_savvy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\NAUKA\Python Nauka\data_science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49162ACC-BDF3-41E6-8474-E396535D9318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1170375A-0BFC-475E-8DA9-AB4AFF963870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="5490" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -356,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D136"/>
+  <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="A137" sqref="A137"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2271,6 +2271,20 @@
         <v>1680</v>
       </c>
     </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>45156</v>
+      </c>
+      <c r="B137" s="2">
+        <v>0.48001157407407408</v>
+      </c>
+      <c r="C137">
+        <v>77977</v>
+      </c>
+      <c r="D137">
+        <v>1680</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more data for disk_savvy and sullygnome
</commit_message>
<xml_diff>
--- a/disk_savvy.xlsx
+++ b/disk_savvy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\NAUKA\Python Nauka\data_science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1170375A-0BFC-475E-8DA9-AB4AFF963870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA5B64C-832E-4A30-9A4C-3C4F4BE57F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="5490" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="75" yWindow="60" windowWidth="5490" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -356,15 +356,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D137"/>
+  <dimension ref="A1:D161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="A138" sqref="A138"/>
+    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="A162" sqref="A162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2285,6 +2288,342 @@
         <v>1680</v>
       </c>
     </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <v>45157</v>
+      </c>
+      <c r="B138" s="2">
+        <v>0.46447916666666672</v>
+      </c>
+      <c r="C138">
+        <v>77983</v>
+      </c>
+      <c r="D138">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <v>45158</v>
+      </c>
+      <c r="B139" s="2">
+        <v>0.46090277777777783</v>
+      </c>
+      <c r="C139">
+        <v>77983</v>
+      </c>
+      <c r="D139">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <v>45159</v>
+      </c>
+      <c r="B140" s="2">
+        <v>0.37771990740740741</v>
+      </c>
+      <c r="C140">
+        <v>77983</v>
+      </c>
+      <c r="D140">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
+        <v>45160</v>
+      </c>
+      <c r="B141" s="2">
+        <v>0.46681712962962968</v>
+      </c>
+      <c r="C141">
+        <v>78041</v>
+      </c>
+      <c r="D141">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <v>45161</v>
+      </c>
+      <c r="B142" s="2">
+        <v>0.46094907407407404</v>
+      </c>
+      <c r="C142">
+        <v>78041</v>
+      </c>
+      <c r="D142">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <v>45162</v>
+      </c>
+      <c r="B143" s="2">
+        <v>0.46054398148148151</v>
+      </c>
+      <c r="C143">
+        <v>78178</v>
+      </c>
+      <c r="D143">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>45163</v>
+      </c>
+      <c r="B144" s="2">
+        <v>0.4636805555555556</v>
+      </c>
+      <c r="C144">
+        <v>78180</v>
+      </c>
+      <c r="D144">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <v>45164</v>
+      </c>
+      <c r="B145" s="2">
+        <v>0.47665509259259259</v>
+      </c>
+      <c r="C145">
+        <v>78180</v>
+      </c>
+      <c r="D145">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <v>45165</v>
+      </c>
+      <c r="B146" s="2">
+        <v>0.46444444444444444</v>
+      </c>
+      <c r="C146">
+        <v>78187</v>
+      </c>
+      <c r="D146">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <v>45166</v>
+      </c>
+      <c r="B147" s="2">
+        <v>0.46377314814814818</v>
+      </c>
+      <c r="C147">
+        <v>78191</v>
+      </c>
+      <c r="D147">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
+        <v>45167</v>
+      </c>
+      <c r="B148" s="2">
+        <v>0.37917824074074075</v>
+      </c>
+      <c r="C148">
+        <v>78212</v>
+      </c>
+      <c r="D148">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
+        <v>45168</v>
+      </c>
+      <c r="B149" s="2">
+        <v>0.46304398148148151</v>
+      </c>
+      <c r="C149">
+        <v>78242</v>
+      </c>
+      <c r="D149">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="1">
+        <v>45169</v>
+      </c>
+      <c r="B150" s="2">
+        <v>0.46733796296296298</v>
+      </c>
+      <c r="C150">
+        <v>78306</v>
+      </c>
+      <c r="D150">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="1">
+        <v>45170</v>
+      </c>
+      <c r="B151" s="2">
+        <v>0.46157407407407408</v>
+      </c>
+      <c r="C151">
+        <v>78316</v>
+      </c>
+      <c r="D151">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="1">
+        <v>45171</v>
+      </c>
+      <c r="B152" s="2">
+        <v>0.46012731481481484</v>
+      </c>
+      <c r="C152">
+        <v>78325</v>
+      </c>
+      <c r="D152">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="1">
+        <v>45172</v>
+      </c>
+      <c r="B153" s="2">
+        <v>0.46033564814814815</v>
+      </c>
+      <c r="C153">
+        <v>78325</v>
+      </c>
+      <c r="D153">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="1">
+        <v>45173</v>
+      </c>
+      <c r="B154" s="2">
+        <v>0.46032407407407411</v>
+      </c>
+      <c r="C154">
+        <v>78368</v>
+      </c>
+      <c r="D154">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="1">
+        <v>45174</v>
+      </c>
+      <c r="B155" s="2">
+        <v>0.46274305555555556</v>
+      </c>
+      <c r="C155">
+        <v>78368</v>
+      </c>
+      <c r="D155">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="1">
+        <v>45175</v>
+      </c>
+      <c r="B156" s="2">
+        <v>0.39006944444444441</v>
+      </c>
+      <c r="C156">
+        <v>78369</v>
+      </c>
+      <c r="D156">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="1">
+        <v>45176</v>
+      </c>
+      <c r="B157" s="2">
+        <v>0.51321759259259259</v>
+      </c>
+      <c r="C157">
+        <v>78374</v>
+      </c>
+      <c r="D157">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
+        <v>45177</v>
+      </c>
+      <c r="B158" s="2">
+        <v>0.46203703703703702</v>
+      </c>
+      <c r="C158">
+        <v>79071</v>
+      </c>
+      <c r="D158">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="1">
+        <v>45178</v>
+      </c>
+      <c r="B159" s="2">
+        <v>0.44128472222222226</v>
+      </c>
+      <c r="C159">
+        <v>79115</v>
+      </c>
+      <c r="D159">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <v>45179</v>
+      </c>
+      <c r="B160" s="2">
+        <v>0.4636805555555556</v>
+      </c>
+      <c r="C160">
+        <v>79115</v>
+      </c>
+      <c r="D160">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="1">
+        <v>45180</v>
+      </c>
+      <c r="B161" s="2">
+        <v>0.46097222222222217</v>
+      </c>
+      <c r="C161">
+        <v>79119</v>
+      </c>
+      <c r="D161">
+        <v>1690</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more disk_savvy data, datacamp practice data
</commit_message>
<xml_diff>
--- a/disk_savvy.xlsx
+++ b/disk_savvy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\NAUKA\Python Nauka\data_science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B942C9-0D58-444E-A8C9-4988C58C17F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024734F5-6E98-490F-B9C4-28FE8D397651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="75" yWindow="60" windowWidth="5490" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -356,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D166"/>
+  <dimension ref="A1:D167"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="A167" sqref="A167"/>
+      <selection activeCell="A168" sqref="A168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2694,6 +2694,20 @@
         <v>1690</v>
       </c>
     </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="1">
+        <v>45186</v>
+      </c>
+      <c r="B167" s="2">
+        <v>0.42137731481481483</v>
+      </c>
+      <c r="C167">
+        <v>84303</v>
+      </c>
+      <c r="D167">
+        <v>1690</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>